<commit_message>
Ya acepta espacios en cadenas y en comentarios
</commit_message>
<xml_diff>
--- a/datos/lenguaje.xlsx
+++ b/datos/lenguaje.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13644" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13740" uniqueCount="176">
   <si>
     <t>ESTADO</t>
   </si>
@@ -550,6 +550,9 @@
   <si>
     <t>231</t>
   </si>
+  <si>
+    <t>232</t>
+  </si>
 </sst>
 </file>
 
@@ -963,13 +966,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CT232"/>
+  <dimension ref="A1:CT233"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BY212" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A139" sqref="A139:XFD139"/>
+      <selection pane="bottomRight" activeCell="CT232" sqref="CT232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69142,9 +69145,303 @@
         <v>86</v>
       </c>
       <c r="CS232" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="CT232" s="7"/>
+    </row>
+    <row r="233" spans="1:98" x14ac:dyDescent="0.25">
+      <c r="A233" s="12">
+        <v>232</v>
+      </c>
+      <c r="B233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="L233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="R233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="S233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="U233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="V233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="W233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="X233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AY233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BA233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BB233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BD233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BE233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BG233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BI233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BJ233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BK233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BL233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BM233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BN233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BO233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BP233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BQ233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BR233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BS233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BT233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BU233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BV233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BW233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BX233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BY233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BZ233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CA233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CB233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CC233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CD233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CE233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CF233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CG233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CH233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CI233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CK233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CL233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CM233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CN233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CO233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CP233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CQ233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CR233" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="CS233" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="CT232" s="7" t="s">
+      <c r="CT233" s="7" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>